<commit_message>
add feature read case data by txt
</commit_message>
<xml_diff>
--- a/datas/excel/platform.xlsx
+++ b/datas/excel/platform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15240" windowHeight="7065"/>
+    <workbookView windowWidth="16920" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>expect</t>
-  </si>
-  <si>
-    <t>result</t>
   </si>
   <si>
     <t>normal</t>
@@ -132,10 +129,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -146,8 +143,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,21 +174,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -177,68 +197,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,10 +212,33 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -268,23 +250,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,25 +296,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,25 +422,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,121 +446,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,11 +490,47 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,17 +550,29 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -542,54 +587,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -598,10 +595,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -610,133 +607,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1098,7 +1095,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
@@ -1114,7 +1111,7 @@
     <col min="10" max="10" width="80.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1144,9 +1141,6 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1154,25 +1148,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1180,25 +1174,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>20</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1206,25 +1200,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1232,25 +1226,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>26</v>
-      </c>
-      <c r="J5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1258,25 +1252,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>29</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1284,25 +1278,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>32</v>
-      </c>
-      <c r="J7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1310,25 +1304,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>35</v>
-      </c>
-      <c r="J8" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>